<commit_message>
updated raw data with FNDR for treatment, and worked with fecundity data to figure out cut-off for days with data
</commit_message>
<xml_diff>
--- a/raw_data/cpb_tei_fecundity_data.xlsx
+++ b/raw_data/cpb_tei_fecundity_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/active_projects/CPB_Phenotype/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8EA6DB-70AB-D943-9D17-A1FEEAF06B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619E7FF6-7D3B-3F4B-B863-210FEDD392D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12047" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12301" uniqueCount="122">
   <si>
     <t>date</t>
   </si>
@@ -760,7 +760,7 @@
   <dimension ref="A1:I2043"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="A832" sqref="A1:A1048576"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -818,7 +818,9 @@
       <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H2" s="8">
         <v>45</v>
       </c>
@@ -845,7 +847,9 @@
       <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H3" s="8">
         <v>86</v>
       </c>
@@ -872,7 +876,9 @@
       <c r="F4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H4" s="8">
         <v>67</v>
       </c>
@@ -899,7 +905,9 @@
       <c r="F5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H5" s="8">
         <v>101</v>
       </c>
@@ -926,7 +934,9 @@
       <c r="F6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H6" s="8">
         <v>76</v>
       </c>
@@ -953,7 +963,9 @@
       <c r="F7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H7" s="8">
         <v>90</v>
       </c>
@@ -980,7 +992,9 @@
       <c r="F8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H8" s="8">
         <v>81</v>
       </c>
@@ -1007,7 +1021,9 @@
       <c r="F9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H9" s="8">
         <v>68</v>
       </c>
@@ -1034,7 +1050,9 @@
       <c r="F10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="8"/>
+      <c r="G10" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H10" s="8">
         <v>88</v>
       </c>
@@ -1061,7 +1079,9 @@
       <c r="F11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="8"/>
+      <c r="G11" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H11" s="8">
         <v>91</v>
       </c>
@@ -1088,7 +1108,9 @@
       <c r="F12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="8"/>
+      <c r="G12" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H12" s="8">
         <v>77</v>
       </c>
@@ -1115,7 +1137,9 @@
       <c r="F13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="8"/>
+      <c r="G13" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H13" s="8">
         <v>37</v>
       </c>
@@ -1142,7 +1166,9 @@
       <c r="F14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="8"/>
+      <c r="G14" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H14" s="8">
         <v>81</v>
       </c>
@@ -1169,7 +1195,9 @@
       <c r="F15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="8"/>
+      <c r="G15" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H15" s="8">
         <v>9</v>
       </c>
@@ -1196,7 +1224,9 @@
       <c r="F16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="8"/>
+      <c r="G16" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H16" s="8">
         <v>75</v>
       </c>
@@ -1223,7 +1253,9 @@
       <c r="F17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="8"/>
+      <c r="G17" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H17" s="8">
         <v>49</v>
       </c>
@@ -1250,7 +1282,9 @@
       <c r="F18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="G18" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H18" s="8">
         <v>0</v>
       </c>
@@ -1277,7 +1311,9 @@
       <c r="F19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="8"/>
+      <c r="G19" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H19" s="8">
         <v>55</v>
       </c>
@@ -1304,7 +1340,9 @@
       <c r="F20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="8"/>
+      <c r="G20" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H20" s="8">
         <v>57</v>
       </c>
@@ -1331,7 +1369,9 @@
       <c r="F21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="8"/>
+      <c r="G21" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H21" s="8">
         <v>26</v>
       </c>
@@ -1358,7 +1398,9 @@
       <c r="F22" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="8"/>
+      <c r="G22" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H22" s="8">
         <v>99</v>
       </c>
@@ -1385,7 +1427,9 @@
       <c r="F23" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="8"/>
+      <c r="G23" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H23" s="8">
         <v>50</v>
       </c>
@@ -1412,7 +1456,9 @@
       <c r="F24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="8"/>
+      <c r="G24" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H24" s="8">
         <v>23</v>
       </c>
@@ -1439,7 +1485,9 @@
       <c r="F25" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="8"/>
+      <c r="G25" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H25" s="8">
         <v>40</v>
       </c>
@@ -1466,7 +1514,9 @@
       <c r="F26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="8"/>
+      <c r="G26" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H26" s="8">
         <v>50</v>
       </c>
@@ -1493,7 +1543,9 @@
       <c r="F27" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="8"/>
+      <c r="G27" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H27" s="8">
         <v>21</v>
       </c>
@@ -1520,7 +1572,9 @@
       <c r="F28" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="8"/>
+      <c r="G28" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H28" s="8">
         <v>93</v>
       </c>
@@ -1547,7 +1601,9 @@
       <c r="F29" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="8"/>
+      <c r="G29" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H29" s="8">
         <v>65</v>
       </c>
@@ -1574,7 +1630,9 @@
       <c r="F30" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="8"/>
+      <c r="G30" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H30" s="8">
         <v>37</v>
       </c>
@@ -1601,7 +1659,9 @@
       <c r="F31" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="8"/>
+      <c r="G31" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H31" s="8">
         <v>56</v>
       </c>
@@ -1628,7 +1688,9 @@
       <c r="F32" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="8"/>
+      <c r="G32" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H32" s="8">
         <v>24</v>
       </c>
@@ -1655,7 +1717,9 @@
       <c r="F33" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="8"/>
+      <c r="G33" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H33" s="8">
         <v>67</v>
       </c>
@@ -1682,7 +1746,9 @@
       <c r="F34" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="8"/>
+      <c r="G34" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H34" s="8">
         <v>55</v>
       </c>
@@ -1709,7 +1775,9 @@
       <c r="F35" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G35" s="8"/>
+      <c r="G35" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H35" s="8">
         <v>0</v>
       </c>
@@ -1736,7 +1804,9 @@
       <c r="F36" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G36" s="8"/>
+      <c r="G36" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H36" s="8">
         <v>0</v>
       </c>
@@ -1763,7 +1833,9 @@
       <c r="F37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="8"/>
+      <c r="G37" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H37" s="8">
         <v>9</v>
       </c>
@@ -1790,7 +1862,9 @@
       <c r="F38" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G38" s="8"/>
+      <c r="G38" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H38" s="8">
         <v>27</v>
       </c>
@@ -1817,7 +1891,9 @@
       <c r="F39" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G39" s="8"/>
+      <c r="G39" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H39" s="8">
         <v>21</v>
       </c>
@@ -1844,7 +1920,9 @@
       <c r="F40" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="8"/>
+      <c r="G40" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H40" s="8">
         <v>54</v>
       </c>
@@ -1871,7 +1949,9 @@
       <c r="F41" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G41" s="8"/>
+      <c r="G41" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H41" s="8">
         <v>63</v>
       </c>
@@ -1898,7 +1978,9 @@
       <c r="F42" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G42" s="8"/>
+      <c r="G42" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H42" s="8">
         <v>12</v>
       </c>
@@ -1925,7 +2007,9 @@
       <c r="F43" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="8"/>
+      <c r="G43" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H43" s="8">
         <v>29</v>
       </c>
@@ -1952,7 +2036,9 @@
       <c r="F44" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G44" s="8"/>
+      <c r="G44" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H44" s="8">
         <v>87</v>
       </c>
@@ -1979,7 +2065,9 @@
       <c r="F45" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G45" s="8"/>
+      <c r="G45" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H45" s="8">
         <v>0</v>
       </c>
@@ -2006,7 +2094,9 @@
       <c r="F46" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G46" s="8"/>
+      <c r="G46" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H46" s="8">
         <v>51</v>
       </c>
@@ -2033,7 +2123,9 @@
       <c r="F47" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G47" s="8"/>
+      <c r="G47" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H47" s="8">
         <v>40</v>
       </c>
@@ -2060,7 +2152,9 @@
       <c r="F48" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G48" s="8"/>
+      <c r="G48" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H48" s="8">
         <v>43</v>
       </c>
@@ -2087,7 +2181,9 @@
       <c r="F49" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G49" s="8"/>
+      <c r="G49" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H49" s="8">
         <v>62</v>
       </c>
@@ -2114,7 +2210,9 @@
       <c r="F50" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G50" s="8"/>
+      <c r="G50" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H50" s="8">
         <v>0</v>
       </c>
@@ -2141,7 +2239,9 @@
       <c r="F51" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G51" s="8"/>
+      <c r="G51" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H51" s="8">
         <v>0</v>
       </c>
@@ -2168,7 +2268,9 @@
       <c r="F52" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G52" s="8"/>
+      <c r="G52" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H52" s="8">
         <v>0</v>
       </c>
@@ -2195,7 +2297,9 @@
       <c r="F53" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G53" s="8"/>
+      <c r="G53" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H53" s="8">
         <v>24</v>
       </c>
@@ -2222,7 +2326,9 @@
       <c r="F54" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G54" s="8"/>
+      <c r="G54" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H54" s="8">
         <v>30</v>
       </c>
@@ -2249,7 +2355,9 @@
       <c r="F55" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G55" s="8"/>
+      <c r="G55" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H55" s="8">
         <v>42</v>
       </c>
@@ -2276,7 +2384,9 @@
       <c r="F56" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G56" s="8"/>
+      <c r="G56" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H56" s="8">
         <v>41</v>
       </c>
@@ -2303,7 +2413,9 @@
       <c r="F57" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G57" s="8"/>
+      <c r="G57" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H57" s="8">
         <v>52</v>
       </c>
@@ -2330,7 +2442,9 @@
       <c r="F58" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G58" s="8"/>
+      <c r="G58" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H58" s="8">
         <v>56</v>
       </c>
@@ -2357,7 +2471,9 @@
       <c r="F59" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G59" s="8"/>
+      <c r="G59" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H59" s="8">
         <v>46</v>
       </c>
@@ -2384,7 +2500,9 @@
       <c r="F60" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G60" s="8"/>
+      <c r="G60" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H60" s="8">
         <v>61</v>
       </c>
@@ -2411,7 +2529,9 @@
       <c r="F61" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G61" s="8"/>
+      <c r="G61" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H61" s="8">
         <v>43</v>
       </c>
@@ -2438,7 +2558,9 @@
       <c r="F62" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G62" s="8"/>
+      <c r="G62" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H62" s="8">
         <v>44</v>
       </c>
@@ -2465,7 +2587,9 @@
       <c r="F63" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G63" s="8"/>
+      <c r="G63" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H63" s="8">
         <v>71</v>
       </c>
@@ -2492,7 +2616,9 @@
       <c r="F64" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G64" s="8"/>
+      <c r="G64" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H64" s="8">
         <v>49</v>
       </c>
@@ -2519,7 +2645,9 @@
       <c r="F65" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G65" s="8"/>
+      <c r="G65" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H65" s="8">
         <v>8</v>
       </c>
@@ -2546,7 +2674,9 @@
       <c r="F66" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G66" s="8"/>
+      <c r="G66" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H66" s="8">
         <v>51</v>
       </c>
@@ -2573,7 +2703,9 @@
       <c r="F67" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G67" s="8"/>
+      <c r="G67" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H67" s="8">
         <v>58</v>
       </c>
@@ -2600,7 +2732,9 @@
       <c r="F68" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G68" s="8"/>
+      <c r="G68" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H68" s="8">
         <v>97</v>
       </c>
@@ -2627,7 +2761,9 @@
       <c r="F69" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G69" s="8"/>
+      <c r="G69" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H69" s="8">
         <v>39</v>
       </c>
@@ -2654,7 +2790,9 @@
       <c r="F70" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G70" s="8"/>
+      <c r="G70" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H70" s="8">
         <v>65</v>
       </c>
@@ -2681,7 +2819,9 @@
       <c r="F71" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G71" s="8"/>
+      <c r="G71" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H71" s="8">
         <v>26</v>
       </c>
@@ -2708,7 +2848,9 @@
       <c r="F72" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G72" s="8"/>
+      <c r="G72" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H72" s="8">
         <v>38</v>
       </c>
@@ -2735,7 +2877,9 @@
       <c r="F73" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G73" s="8"/>
+      <c r="G73" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H73" s="8">
         <v>90</v>
       </c>
@@ -2762,7 +2906,9 @@
       <c r="F74" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G74" s="8"/>
+      <c r="G74" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H74" s="8">
         <v>0</v>
       </c>
@@ -2789,7 +2935,9 @@
       <c r="F75" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G75" s="8"/>
+      <c r="G75" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H75" s="8">
         <v>42</v>
       </c>
@@ -2816,7 +2964,9 @@
       <c r="F76" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G76" s="8"/>
+      <c r="G76" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H76" s="8">
         <v>50</v>
       </c>
@@ -2843,7 +2993,9 @@
       <c r="F77" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G77" s="8"/>
+      <c r="G77" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H77" s="8">
         <v>29</v>
       </c>
@@ -2870,7 +3022,9 @@
       <c r="F78" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G78" s="8"/>
+      <c r="G78" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H78" s="8">
         <v>51</v>
       </c>
@@ -2897,7 +3051,9 @@
       <c r="F79" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G79" s="8"/>
+      <c r="G79" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H79" s="8">
         <v>12</v>
       </c>
@@ -2924,7 +3080,9 @@
       <c r="F80" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G80" s="8"/>
+      <c r="G80" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H80" s="8">
         <v>44</v>
       </c>
@@ -2951,7 +3109,9 @@
       <c r="F81" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G81" s="8"/>
+      <c r="G81" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H81" s="8">
         <v>72</v>
       </c>
@@ -2978,7 +3138,9 @@
       <c r="F82" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G82" s="8"/>
+      <c r="G82" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H82" s="8">
         <v>88</v>
       </c>
@@ -3005,7 +3167,9 @@
       <c r="F83" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G83" s="8"/>
+      <c r="G83" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H83" s="8">
         <v>82</v>
       </c>
@@ -3032,7 +3196,9 @@
       <c r="F84" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G84" s="8"/>
+      <c r="G84" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H84" s="8">
         <v>71</v>
       </c>
@@ -3059,7 +3225,9 @@
       <c r="F85" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G85" s="8"/>
+      <c r="G85" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H85" s="8">
         <v>120</v>
       </c>
@@ -3086,7 +3254,9 @@
       <c r="F86" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G86" s="8"/>
+      <c r="G86" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H86" s="8">
         <v>19</v>
       </c>
@@ -3113,7 +3283,9 @@
       <c r="F87" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G87" s="8"/>
+      <c r="G87" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H87" s="8">
         <v>64</v>
       </c>
@@ -3140,7 +3312,9 @@
       <c r="F88" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G88" s="8"/>
+      <c r="G88" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H88" s="8">
         <v>64</v>
       </c>
@@ -3167,7 +3341,9 @@
       <c r="F89" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G89" s="8"/>
+      <c r="G89" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H89" s="8">
         <v>120</v>
       </c>
@@ -3194,7 +3370,9 @@
       <c r="F90" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G90" s="8"/>
+      <c r="G90" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H90" s="8">
         <v>20</v>
       </c>
@@ -3221,7 +3399,9 @@
       <c r="F91" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G91" s="8"/>
+      <c r="G91" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H91" s="8">
         <v>0</v>
       </c>
@@ -3248,7 +3428,9 @@
       <c r="F92" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G92" s="8"/>
+      <c r="G92" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H92" s="8">
         <v>0</v>
       </c>
@@ -3275,7 +3457,9 @@
       <c r="F93" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G93" s="8"/>
+      <c r="G93" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H93" s="8">
         <v>30</v>
       </c>
@@ -3302,7 +3486,9 @@
       <c r="F94" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G94" s="8"/>
+      <c r="G94" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H94" s="8">
         <v>32</v>
       </c>
@@ -3329,7 +3515,9 @@
       <c r="F95" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G95" s="8"/>
+      <c r="G95" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H95" s="8">
         <v>47</v>
       </c>
@@ -3356,7 +3544,9 @@
       <c r="F96" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G96" s="8"/>
+      <c r="G96" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H96" s="8">
         <v>47</v>
       </c>
@@ -3383,7 +3573,9 @@
       <c r="F97" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G97" s="8"/>
+      <c r="G97" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H97" s="8">
         <v>70</v>
       </c>
@@ -3410,7 +3602,9 @@
       <c r="F98" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G98" s="8"/>
+      <c r="G98" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H98" s="8">
         <v>84</v>
       </c>
@@ -3437,7 +3631,9 @@
       <c r="F99" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G99" s="8"/>
+      <c r="G99" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H99" s="8">
         <v>58</v>
       </c>
@@ -3464,7 +3660,9 @@
       <c r="F100" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G100" s="8"/>
+      <c r="G100" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H100" s="8">
         <v>80</v>
       </c>
@@ -3491,7 +3689,9 @@
       <c r="F101" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G101" s="8"/>
+      <c r="G101" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H101" s="8">
         <v>36</v>
       </c>
@@ -3518,7 +3718,9 @@
       <c r="F102" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G102" s="8"/>
+      <c r="G102" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H102" s="8">
         <v>89</v>
       </c>
@@ -3545,7 +3747,9 @@
       <c r="F103" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G103" s="8"/>
+      <c r="G103" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H103" s="8">
         <v>58</v>
       </c>
@@ -3572,7 +3776,9 @@
       <c r="F104" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G104" s="8"/>
+      <c r="G104" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H104" s="8">
         <v>35</v>
       </c>
@@ -3599,7 +3805,9 @@
       <c r="F105" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G105" s="8"/>
+      <c r="G105" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H105" s="8">
         <v>30</v>
       </c>
@@ -3626,7 +3834,9 @@
       <c r="F106" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G106" s="8"/>
+      <c r="G106" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H106" s="8">
         <v>52</v>
       </c>
@@ -3653,7 +3863,9 @@
       <c r="F107" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G107" s="8"/>
+      <c r="G107" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H107" s="8">
         <v>26</v>
       </c>
@@ -3680,7 +3892,9 @@
       <c r="F108" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G108" s="8"/>
+      <c r="G108" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H108" s="8">
         <v>106</v>
       </c>
@@ -3707,7 +3921,9 @@
       <c r="F109" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G109" s="8"/>
+      <c r="G109" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H109" s="8">
         <v>50</v>
       </c>
@@ -3734,7 +3950,9 @@
       <c r="F110" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G110" s="8"/>
+      <c r="G110" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H110" s="8">
         <v>38</v>
       </c>
@@ -3761,7 +3979,9 @@
       <c r="F111" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G111" s="8"/>
+      <c r="G111" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H111" s="8">
         <v>43</v>
       </c>
@@ -3788,7 +4008,9 @@
       <c r="F112" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G112" s="8"/>
+      <c r="G112" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H112" s="8">
         <v>55</v>
       </c>
@@ -3815,7 +4037,9 @@
       <c r="F113" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G113" s="8"/>
+      <c r="G113" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H113" s="8">
         <v>52</v>
       </c>
@@ -3842,7 +4066,9 @@
       <c r="F114" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G114" s="8"/>
+      <c r="G114" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H114" s="8">
         <v>66</v>
       </c>
@@ -3869,7 +4095,9 @@
       <c r="F115" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G115" s="8"/>
+      <c r="G115" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H115" s="8">
         <v>33</v>
       </c>
@@ -3896,7 +4124,9 @@
       <c r="F116" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G116" s="8"/>
+      <c r="G116" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H116" s="8">
         <v>29</v>
       </c>
@@ -3923,7 +4153,9 @@
       <c r="F117" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G117" s="8"/>
+      <c r="G117" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H117" s="8">
         <v>36</v>
       </c>
@@ -3950,7 +4182,9 @@
       <c r="F118" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G118" s="8"/>
+      <c r="G118" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H118" s="8">
         <v>46</v>
       </c>
@@ -3977,7 +4211,9 @@
       <c r="F119" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G119" s="8"/>
+      <c r="G119" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H119" s="8">
         <v>0</v>
       </c>
@@ -4004,7 +4240,9 @@
       <c r="F120" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G120" s="8"/>
+      <c r="G120" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H120" s="8">
         <v>71</v>
       </c>
@@ -4031,7 +4269,9 @@
       <c r="F121" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G121" s="8"/>
+      <c r="G121" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H121" s="8">
         <v>73</v>
       </c>
@@ -4058,7 +4298,9 @@
       <c r="F122" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G122" s="8"/>
+      <c r="G122" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H122" s="8">
         <v>64</v>
       </c>
@@ -4085,7 +4327,9 @@
       <c r="F123" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G123" s="8"/>
+      <c r="G123" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H123" s="8">
         <v>120</v>
       </c>
@@ -4112,7 +4356,9 @@
       <c r="F124" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G124" s="8"/>
+      <c r="G124" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H124" s="8">
         <v>60</v>
       </c>
@@ -4139,7 +4385,9 @@
       <c r="F125" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G125" s="8"/>
+      <c r="G125" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H125" s="8">
         <v>11</v>
       </c>
@@ -4166,7 +4414,9 @@
       <c r="F126" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G126" s="8"/>
+      <c r="G126" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H126" s="8">
         <v>57</v>
       </c>
@@ -4193,7 +4443,9 @@
       <c r="F127" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G127" s="8"/>
+      <c r="G127" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H127" s="8">
         <v>43</v>
       </c>
@@ -4220,7 +4472,9 @@
       <c r="F128" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G128" s="8"/>
+      <c r="G128" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H128" s="8">
         <v>24</v>
       </c>
@@ -4247,7 +4501,9 @@
       <c r="F129" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G129" s="8"/>
+      <c r="G129" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H129" s="8">
         <v>27</v>
       </c>
@@ -4274,7 +4530,9 @@
       <c r="F130" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G130" s="8"/>
+      <c r="G130" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H130" s="8">
         <v>30</v>
       </c>
@@ -4301,7 +4559,9 @@
       <c r="F131" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G131" s="8"/>
+      <c r="G131" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H131" s="8">
         <v>0</v>
       </c>
@@ -4328,7 +4588,9 @@
       <c r="F132" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G132" s="8"/>
+      <c r="G132" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H132" s="8">
         <v>0</v>
       </c>
@@ -4355,7 +4617,9 @@
       <c r="F133" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G133" s="8"/>
+      <c r="G133" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H133" s="8">
         <v>0</v>
       </c>
@@ -4382,7 +4646,9 @@
       <c r="F134" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G134" s="8"/>
+      <c r="G134" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H134" s="8">
         <v>56</v>
       </c>
@@ -4409,7 +4675,9 @@
       <c r="F135" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G135" s="8"/>
+      <c r="G135" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H135" s="8">
         <v>0</v>
       </c>
@@ -4436,7 +4704,9 @@
       <c r="F136" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G136" s="8"/>
+      <c r="G136" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H136" s="8">
         <v>36</v>
       </c>
@@ -4463,7 +4733,9 @@
       <c r="F137" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G137" s="8"/>
+      <c r="G137" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H137" s="8">
         <v>57</v>
       </c>
@@ -4490,7 +4762,9 @@
       <c r="F138" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G138" s="8"/>
+      <c r="G138" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H138" s="8">
         <v>42</v>
       </c>
@@ -4517,7 +4791,9 @@
       <c r="F139" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G139" s="8"/>
+      <c r="G139" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H139" s="8">
         <v>31</v>
       </c>
@@ -4544,7 +4820,9 @@
       <c r="F140" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G140" s="8"/>
+      <c r="G140" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H140" s="8">
         <v>6</v>
       </c>
@@ -4571,7 +4849,9 @@
       <c r="F141" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G141" s="8"/>
+      <c r="G141" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H141" s="8">
         <v>41</v>
       </c>
@@ -4598,7 +4878,9 @@
       <c r="F142" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G142" s="8"/>
+      <c r="G142" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H142" s="8">
         <v>0</v>
       </c>
@@ -4625,7 +4907,9 @@
       <c r="F143" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G143" s="8"/>
+      <c r="G143" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H143" s="8">
         <v>42</v>
       </c>
@@ -4652,7 +4936,9 @@
       <c r="F144" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G144" s="8"/>
+      <c r="G144" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H144" s="8">
         <v>33</v>
       </c>
@@ -4679,7 +4965,9 @@
       <c r="F145" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G145" s="8"/>
+      <c r="G145" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H145" s="8">
         <v>41</v>
       </c>
@@ -4706,7 +4994,9 @@
       <c r="F146" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G146" s="8"/>
+      <c r="G146" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H146" s="8">
         <v>52</v>
       </c>
@@ -4733,7 +5023,9 @@
       <c r="F147" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G147" s="8"/>
+      <c r="G147" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H147" s="8">
         <v>83</v>
       </c>
@@ -4760,7 +5052,9 @@
       <c r="F148" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G148" s="8"/>
+      <c r="G148" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H148" s="8">
         <v>63</v>
       </c>
@@ -4787,7 +5081,9 @@
       <c r="F149" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G149" s="8"/>
+      <c r="G149" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H149" s="8">
         <v>66</v>
       </c>
@@ -4814,7 +5110,9 @@
       <c r="F150" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G150" s="8"/>
+      <c r="G150" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H150" s="8">
         <v>37</v>
       </c>
@@ -4841,7 +5139,9 @@
       <c r="F151" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G151" s="8"/>
+      <c r="G151" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H151" s="8">
         <v>52</v>
       </c>
@@ -4868,7 +5168,9 @@
       <c r="F152" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G152" s="8"/>
+      <c r="G152" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H152" s="8">
         <v>56</v>
       </c>
@@ -4895,7 +5197,9 @@
       <c r="F153" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G153" s="8"/>
+      <c r="G153" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H153" s="8">
         <v>0</v>
       </c>
@@ -4922,7 +5226,9 @@
       <c r="F154" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G154" s="8"/>
+      <c r="G154" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H154" s="8">
         <v>56</v>
       </c>
@@ -4949,7 +5255,9 @@
       <c r="F155" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G155" s="8"/>
+      <c r="G155" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H155" s="8">
         <v>14</v>
       </c>
@@ -4976,7 +5284,9 @@
       <c r="F156" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G156" s="8"/>
+      <c r="G156" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H156" s="8">
         <v>75</v>
       </c>
@@ -5003,7 +5313,9 @@
       <c r="F157" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G157" s="8"/>
+      <c r="G157" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H157" s="8">
         <v>42</v>
       </c>
@@ -5030,7 +5342,9 @@
       <c r="F158" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G158" s="8"/>
+      <c r="G158" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H158" s="8">
         <v>28</v>
       </c>
@@ -5057,7 +5371,9 @@
       <c r="F159" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G159" s="8"/>
+      <c r="G159" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H159" s="8">
         <v>39</v>
       </c>
@@ -5084,7 +5400,9 @@
       <c r="F160" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G160" s="8"/>
+      <c r="G160" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H160" s="8">
         <v>34</v>
       </c>
@@ -5111,7 +5429,9 @@
       <c r="F161" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G161" s="8"/>
+      <c r="G161" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H161" s="8">
         <v>41</v>
       </c>
@@ -5138,7 +5458,9 @@
       <c r="F162" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G162" s="8"/>
+      <c r="G162" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H162" s="8">
         <v>16</v>
       </c>
@@ -5165,7 +5487,9 @@
       <c r="F163" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G163" s="8"/>
+      <c r="G163" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H163" s="8">
         <v>0</v>
       </c>
@@ -5192,7 +5516,9 @@
       <c r="F164" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G164" s="8"/>
+      <c r="G164" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H164" s="8">
         <v>104</v>
       </c>
@@ -5219,7 +5545,9 @@
       <c r="F165" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G165" s="8"/>
+      <c r="G165" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H165" s="8">
         <v>20</v>
       </c>
@@ -5246,7 +5574,9 @@
       <c r="F166" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G166" s="8"/>
+      <c r="G166" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H166" s="8">
         <v>44</v>
       </c>
@@ -5273,7 +5603,9 @@
       <c r="F167" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G167" s="8"/>
+      <c r="G167" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H167" s="8">
         <v>16</v>
       </c>
@@ -5300,7 +5632,9 @@
       <c r="F168" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G168" s="8"/>
+      <c r="G168" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H168" s="8">
         <v>64</v>
       </c>
@@ -5327,7 +5661,9 @@
       <c r="F169" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G169" s="8"/>
+      <c r="G169" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H169" s="8">
         <v>0</v>
       </c>
@@ -5354,7 +5690,9 @@
       <c r="F170" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G170" s="8"/>
+      <c r="G170" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H170" s="8">
         <v>125</v>
       </c>
@@ -5381,7 +5719,9 @@
       <c r="F171" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G171" s="8"/>
+      <c r="G171" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H171" s="8">
         <v>71</v>
       </c>
@@ -5408,7 +5748,9 @@
       <c r="F172" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G172" s="8"/>
+      <c r="G172" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H172" s="8">
         <v>56</v>
       </c>
@@ -5435,7 +5777,9 @@
       <c r="F173" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G173" s="8"/>
+      <c r="G173" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H173" s="8">
         <v>117</v>
       </c>
@@ -5462,7 +5806,9 @@
       <c r="F174" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G174" s="8"/>
+      <c r="G174" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H174" s="8">
         <v>74</v>
       </c>
@@ -5489,7 +5835,9 @@
       <c r="F175" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G175" s="8"/>
+      <c r="G175" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H175" s="8">
         <v>0</v>
       </c>
@@ -5516,7 +5864,9 @@
       <c r="F176" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G176" s="8"/>
+      <c r="G176" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H176" s="8">
         <v>65</v>
       </c>
@@ -5543,7 +5893,9 @@
       <c r="F177" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G177" s="8"/>
+      <c r="G177" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H177" s="8">
         <v>133</v>
       </c>
@@ -5570,7 +5922,9 @@
       <c r="F178" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G178" s="8"/>
+      <c r="G178" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H178" s="8">
         <v>52</v>
       </c>
@@ -5597,7 +5951,9 @@
       <c r="F179" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G179" s="8"/>
+      <c r="G179" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H179" s="8">
         <v>110</v>
       </c>
@@ -5624,7 +5980,9 @@
       <c r="F180" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G180" s="8"/>
+      <c r="G180" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H180" s="8">
         <v>0</v>
       </c>
@@ -5651,7 +6009,9 @@
       <c r="F181" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G181" s="8"/>
+      <c r="G181" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H181" s="8">
         <v>123</v>
       </c>
@@ -5678,7 +6038,9 @@
       <c r="F182" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G182" s="8"/>
+      <c r="G182" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H182" s="8">
         <v>31</v>
       </c>
@@ -5705,7 +6067,9 @@
       <c r="F183" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G183" s="8"/>
+      <c r="G183" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H183" s="8">
         <v>124</v>
       </c>
@@ -5732,7 +6096,9 @@
       <c r="F184" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G184" s="8"/>
+      <c r="G184" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H184" s="8">
         <v>34</v>
       </c>
@@ -5759,7 +6125,9 @@
       <c r="F185" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G185" s="8"/>
+      <c r="G185" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H185" s="8">
         <v>65</v>
       </c>
@@ -5786,7 +6154,9 @@
       <c r="F186" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G186" s="8"/>
+      <c r="G186" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H186" s="8">
         <v>123</v>
       </c>
@@ -5813,7 +6183,9 @@
       <c r="F187" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G187" s="8"/>
+      <c r="G187" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H187" s="8">
         <v>63</v>
       </c>
@@ -5840,7 +6212,9 @@
       <c r="F188" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G188" s="8"/>
+      <c r="G188" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H188" s="8">
         <v>36</v>
       </c>
@@ -5867,7 +6241,9 @@
       <c r="F189" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G189" s="8"/>
+      <c r="G189" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H189" s="8">
         <v>75</v>
       </c>
@@ -5894,7 +6270,9 @@
       <c r="F190" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G190" s="8"/>
+      <c r="G190" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H190" s="8">
         <v>10</v>
       </c>
@@ -5921,7 +6299,9 @@
       <c r="F191" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G191" s="8"/>
+      <c r="G191" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H191" s="8">
         <v>90</v>
       </c>
@@ -5948,7 +6328,9 @@
       <c r="F192" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G192" s="8"/>
+      <c r="G192" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H192" s="8">
         <v>0</v>
       </c>
@@ -5975,7 +6357,9 @@
       <c r="F193" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G193" s="8"/>
+      <c r="G193" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H193" s="8">
         <v>0</v>
       </c>
@@ -6002,7 +6386,9 @@
       <c r="F194" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G194" s="8"/>
+      <c r="G194" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H194" s="8">
         <v>0</v>
       </c>
@@ -6029,7 +6415,9 @@
       <c r="F195" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G195" s="8"/>
+      <c r="G195" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H195" s="8">
         <v>8</v>
       </c>
@@ -6056,7 +6444,9 @@
       <c r="F196" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G196" s="8"/>
+      <c r="G196" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H196" s="8">
         <v>29</v>
       </c>
@@ -6083,7 +6473,9 @@
       <c r="F197" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G197" s="8"/>
+      <c r="G197" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H197" s="8">
         <v>0</v>
       </c>
@@ -6110,7 +6502,9 @@
       <c r="F198" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G198" s="8"/>
+      <c r="G198" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H198" s="8">
         <v>100</v>
       </c>
@@ -6137,7 +6531,9 @@
       <c r="F199" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G199" s="8"/>
+      <c r="G199" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H199" s="8">
         <v>39</v>
       </c>
@@ -6164,7 +6560,9 @@
       <c r="F200" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G200" s="8"/>
+      <c r="G200" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H200" s="8">
         <v>0</v>
       </c>
@@ -6191,7 +6589,9 @@
       <c r="F201" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G201" s="8"/>
+      <c r="G201" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H201" s="8">
         <v>0</v>
       </c>
@@ -6218,7 +6618,9 @@
       <c r="F202" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G202" s="8"/>
+      <c r="G202" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H202" s="8">
         <v>91</v>
       </c>
@@ -6245,7 +6647,9 @@
       <c r="F203" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G203" s="8"/>
+      <c r="G203" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H203" s="8">
         <v>50</v>
       </c>
@@ -6272,7 +6676,9 @@
       <c r="F204" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G204" s="8"/>
+      <c r="G204" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H204" s="8">
         <v>50</v>
       </c>
@@ -6299,7 +6705,9 @@
       <c r="F205" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G205" s="8"/>
+      <c r="G205" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H205" s="8">
         <v>64</v>
       </c>
@@ -6326,7 +6734,9 @@
       <c r="F206" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G206" s="8"/>
+      <c r="G206" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H206" s="8">
         <v>74</v>
       </c>
@@ -6353,7 +6763,9 @@
       <c r="F207" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G207" s="8"/>
+      <c r="G207" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H207" s="8">
         <v>86</v>
       </c>
@@ -6380,7 +6792,9 @@
       <c r="F208" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G208" s="8"/>
+      <c r="G208" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H208" s="8">
         <v>78</v>
       </c>
@@ -6407,7 +6821,9 @@
       <c r="F209" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G209" s="8"/>
+      <c r="G209" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H209" s="8">
         <v>78</v>
       </c>
@@ -6434,7 +6850,9 @@
       <c r="F210" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G210" s="8"/>
+      <c r="G210" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H210" s="8">
         <v>136</v>
       </c>
@@ -6461,7 +6879,9 @@
       <c r="F211" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G211" s="8"/>
+      <c r="G211" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H211" s="8">
         <v>91</v>
       </c>
@@ -6488,7 +6908,9 @@
       <c r="F212" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G212" s="8"/>
+      <c r="G212" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H212" s="8">
         <v>90</v>
       </c>
@@ -6515,7 +6937,9 @@
       <c r="F213" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G213" s="8"/>
+      <c r="G213" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H213" s="8">
         <v>84</v>
       </c>
@@ -6542,7 +6966,9 @@
       <c r="F214" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G214" s="8"/>
+      <c r="G214" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H214" s="8">
         <v>83</v>
       </c>
@@ -6569,7 +6995,9 @@
       <c r="F215" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G215" s="8"/>
+      <c r="G215" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H215" s="8">
         <v>51</v>
       </c>
@@ -6596,7 +7024,9 @@
       <c r="F216" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G216" s="8"/>
+      <c r="G216" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H216" s="8">
         <v>72</v>
       </c>
@@ -6623,7 +7053,9 @@
       <c r="F217" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G217" s="8"/>
+      <c r="G217" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H217" s="8">
         <v>126</v>
       </c>
@@ -6650,7 +7082,9 @@
       <c r="F218" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G218" s="8"/>
+      <c r="G218" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H218" s="8">
         <v>77</v>
       </c>
@@ -6677,7 +7111,9 @@
       <c r="F219" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G219" s="8"/>
+      <c r="G219" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H219" s="8">
         <v>36</v>
       </c>
@@ -6704,7 +7140,9 @@
       <c r="F220" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G220" s="8"/>
+      <c r="G220" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H220" s="8">
         <v>75</v>
       </c>
@@ -6731,7 +7169,9 @@
       <c r="F221" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G221" s="8"/>
+      <c r="G221" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H221" s="8">
         <v>0</v>
       </c>
@@ -6758,7 +7198,9 @@
       <c r="F222" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G222" s="8"/>
+      <c r="G222" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H222" s="8">
         <v>56</v>
       </c>
@@ -6785,7 +7227,9 @@
       <c r="F223" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G223" s="8"/>
+      <c r="G223" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H223" s="8">
         <v>37</v>
       </c>
@@ -6812,7 +7256,9 @@
       <c r="F224" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G224" s="8"/>
+      <c r="G224" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H224" s="8">
         <v>0</v>
       </c>
@@ -6839,7 +7285,9 @@
       <c r="F225" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G225" s="8"/>
+      <c r="G225" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H225" s="8">
         <v>0</v>
       </c>
@@ -6866,7 +7314,9 @@
       <c r="F226" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G226" s="8"/>
+      <c r="G226" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H226" s="8">
         <v>45</v>
       </c>
@@ -6893,7 +7343,9 @@
       <c r="F227" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G227" s="8"/>
+      <c r="G227" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H227" s="8">
         <v>75</v>
       </c>
@@ -6920,7 +7372,9 @@
       <c r="F228" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G228" s="8"/>
+      <c r="G228" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H228" s="8">
         <v>0</v>
       </c>
@@ -6947,7 +7401,9 @@
       <c r="F229" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G229" s="8"/>
+      <c r="G229" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H229" s="8">
         <v>145</v>
       </c>
@@ -6974,7 +7430,9 @@
       <c r="F230" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G230" s="8"/>
+      <c r="G230" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H230" s="8">
         <v>65</v>
       </c>
@@ -7001,7 +7459,9 @@
       <c r="F231" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G231" s="8"/>
+      <c r="G231" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H231" s="8">
         <v>99</v>
       </c>
@@ -7028,7 +7488,9 @@
       <c r="F232" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G232" s="8"/>
+      <c r="G232" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H232" s="8">
         <v>82</v>
       </c>
@@ -7055,7 +7517,9 @@
       <c r="F233" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G233" s="8"/>
+      <c r="G233" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H233" s="8">
         <v>64</v>
       </c>
@@ -7082,7 +7546,9 @@
       <c r="F234" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G234" s="8"/>
+      <c r="G234" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H234" s="8">
         <v>45</v>
       </c>
@@ -7109,7 +7575,9 @@
       <c r="F235" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G235" s="8"/>
+      <c r="G235" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H235" s="8">
         <v>61</v>
       </c>
@@ -7136,7 +7604,9 @@
       <c r="F236" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G236" s="8"/>
+      <c r="G236" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H236" s="8">
         <v>82</v>
       </c>
@@ -7163,7 +7633,9 @@
       <c r="F237" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G237" s="8"/>
+      <c r="G237" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H237" s="8">
         <v>70</v>
       </c>
@@ -7190,7 +7662,9 @@
       <c r="F238" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G238" s="8"/>
+      <c r="G238" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H238" s="8">
         <v>0</v>
       </c>
@@ -7217,7 +7691,9 @@
       <c r="F239" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G239" s="8"/>
+      <c r="G239" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H239" s="8">
         <v>117</v>
       </c>
@@ -7244,7 +7720,9 @@
       <c r="F240" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G240" s="8"/>
+      <c r="G240" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H240" s="8">
         <v>0</v>
       </c>
@@ -7271,7 +7749,9 @@
       <c r="F241" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G241" s="8"/>
+      <c r="G241" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H241" s="8">
         <v>71</v>
       </c>
@@ -7298,7 +7778,9 @@
       <c r="F242" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G242" s="8"/>
+      <c r="G242" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H242" s="8">
         <v>85</v>
       </c>
@@ -7325,7 +7807,9 @@
       <c r="F243" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G243" s="8"/>
+      <c r="G243" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H243" s="8">
         <v>88</v>
       </c>
@@ -7352,7 +7836,9 @@
       <c r="F244" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G244" s="8"/>
+      <c r="G244" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H244" s="8">
         <v>70</v>
       </c>
@@ -7379,7 +7865,9 @@
       <c r="F245" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G245" s="8"/>
+      <c r="G245" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H245" s="8">
         <v>34</v>
       </c>
@@ -7406,7 +7894,9 @@
       <c r="F246" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G246" s="8"/>
+      <c r="G246" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H246" s="8">
         <v>83</v>
       </c>
@@ -7433,7 +7923,9 @@
       <c r="F247" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G247" s="8"/>
+      <c r="G247" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H247" s="8">
         <v>71</v>
       </c>
@@ -7460,7 +7952,9 @@
       <c r="F248" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G248" s="8"/>
+      <c r="G248" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H248" s="8">
         <v>0</v>
       </c>
@@ -7487,7 +7981,9 @@
       <c r="F249" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G249" s="8"/>
+      <c r="G249" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H249" s="8">
         <v>0</v>
       </c>
@@ -7514,7 +8010,9 @@
       <c r="F250" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G250" s="8"/>
+      <c r="G250" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H250" s="8">
         <v>28</v>
       </c>
@@ -7541,7 +8039,9 @@
       <c r="F251" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G251" s="8"/>
+      <c r="G251" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H251" s="8">
         <v>36</v>
       </c>
@@ -7568,7 +8068,9 @@
       <c r="F252" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G252" s="8"/>
+      <c r="G252" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H252" s="8">
         <v>59</v>
       </c>
@@ -7595,7 +8097,9 @@
       <c r="F253" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G253" s="8"/>
+      <c r="G253" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H253" s="8">
         <v>124</v>
       </c>
@@ -7622,7 +8126,9 @@
       <c r="F254" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G254" s="8"/>
+      <c r="G254" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H254" s="8">
         <v>0</v>
       </c>
@@ -7649,7 +8155,9 @@
       <c r="F255" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G255" s="8"/>
+      <c r="G255" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H255" s="8">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
finalized analysis of mean fecundity over number of days of fecundity data
</commit_message>
<xml_diff>
--- a/raw_data/cpb_tei_fecundity_data.xlsx
+++ b/raw_data/cpb_tei_fecundity_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/active_projects/CPB_Phenotype/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619E7FF6-7D3B-3F4B-B863-210FEDD392D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7D18D8-A798-644D-891C-AC1CAF6B4C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -760,7 +760,7 @@
   <dimension ref="A1:I2043"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>